<commit_message>
Ajout du champ description pour les tâches et calcul automatique des avancements par catégorie
</commit_message>
<xml_diff>
--- a/Import Tache.xlsx
+++ b/Import Tache.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanchabrerie/Obeya/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC06660-4A33-9B40-A445-3BC45AD223AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA082047-31E0-664E-BA95-53C2FF669C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="660" windowWidth="28040" windowHeight="17160" xr2:uid="{087953B2-9BBB-244C-9FDF-22DC41172B2E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Tâche</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Industrialisation</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Amortisseur</t>
+  </si>
+  <si>
+    <t>Yo</t>
+  </si>
+  <si>
+    <t>Youpi</t>
   </si>
 </sst>
 </file>
@@ -484,20 +496,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EFBEEE-7CE9-3840-AA17-377BD7526902}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,205 +518,217 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>46023</v>
       </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>46024</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2">
         <v>46025</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>46026</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>46027</v>
       </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>46028</v>
       </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>46029</v>
       </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2">
         <v>46030</v>
       </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>46031</v>
       </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>46032</v>
       </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>46033</v>
       </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>46034</v>
       </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2">
         <v>46035</v>
       </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>46036</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>0</v>
       </c>
     </row>
@@ -713,7 +738,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{A07C29E9-5FCF-D547-9586-C41189BD8ACF}">
       <formula1>"Jalon,Livrable,Etude,Prototype,Map-Qual-Val,Industrialisation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15" xr:uid="{D94D65D3-8C1F-EC4B-BA97-A2770B36F83A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15" xr:uid="{D94D65D3-8C1F-EC4B-BA97-A2770B36F83A}">
       <formula1>"0%,50%,100%"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>